<commit_message>
Squash merge framework/feature-SNAPSHOT.20240922 into dev
</commit_message>
<xml_diff>
--- a/assets/Localization-Resources.xlsx
+++ b/assets/Localization-Resources.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="60">
   <si>
     <t>Project</t>
   </si>
@@ -138,6 +138,75 @@
   </si>
   <si>
     <t>无效的方法参数 “{0}” 值：NULL。</t>
+  </si>
+  <si>
+    <t>DateTime_just_now</t>
+  </si>
+  <si>
+    <t>一分钟以内</t>
+  </si>
+  <si>
+    <t>Just now</t>
+  </si>
+  <si>
+    <t>刚刚</t>
+  </si>
+  <si>
+    <t>DateTime_several_minutes_ago</t>
+  </si>
+  <si>
+    <t>60 分钟以内</t>
+  </si>
+  <si>
+    <t>{0} minutes ago</t>
+  </si>
+  <si>
+    <t>{0} 分钟前</t>
+  </si>
+  <si>
+    <t>DateTime_several_hours_ago</t>
+  </si>
+  <si>
+    <t>24 小时以内</t>
+  </si>
+  <si>
+    <t>{0} hours ago</t>
+  </si>
+  <si>
+    <t>{0} 小时前</t>
+  </si>
+  <si>
+    <t>DateTime_several_days_ago</t>
+  </si>
+  <si>
+    <t>30 天以内</t>
+  </si>
+  <si>
+    <t>{0} days ago</t>
+  </si>
+  <si>
+    <t>{0} 天前</t>
+  </si>
+  <si>
+    <t>DateTime_same_year</t>
+  </si>
+  <si>
+    <t>同一年</t>
+  </si>
+  <si>
+    <t>dd/MM</t>
+  </si>
+  <si>
+    <t>MM月dd日</t>
+  </si>
+  <si>
+    <t>DateTime_date_only</t>
+  </si>
+  <si>
+    <t>dd/MM/yyyy</t>
+  </si>
+  <si>
+    <t>yyyy年MM月dd日</t>
   </si>
 </sst>
 </file>
@@ -1329,14 +1398,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10:B12"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="28.3" customHeight="1"/>
@@ -1599,6 +1668,141 @@
         <v>36</v>
       </c>
     </row>
+    <row r="13" customHeight="1" spans="1:9">
+      <c r="A13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" customHeight="1" spans="1:9">
+      <c r="A14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" customHeight="1" spans="1:9">
+      <c r="A15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" customHeight="1" spans="1:9">
+      <c r="A16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" customHeight="1" spans="1:9">
+      <c r="A17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" customHeight="1" spans="1:9">
+      <c r="A18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" sort="0" autoFilter="0"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Squash merge framework/feature-SNAPSHOT.20241005 into dev
</commit_message>
<xml_diff>
--- a/assets/Localization-Resources.xlsx
+++ b/assets/Localization-Resources.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="66">
   <si>
     <t>Project</t>
   </si>
@@ -207,6 +207,24 @@
   </si>
   <si>
     <t>yyyy年MM月dd日</t>
+  </si>
+  <si>
+    <t>ArgumentException_empty_string</t>
+  </si>
+  <si>
+    <t>The string parameter "{0}" is not allowed to be NULL or empty.</t>
+  </si>
+  <si>
+    <t>字符串参数“{0}”不允许为 NULL 或空白。</t>
+  </si>
+  <si>
+    <t>ArgumentException_empty_or_whitespace</t>
+  </si>
+  <si>
+    <t>The string parameter "{0}" is not allowed to be NULL or empty or white-spaces.</t>
+  </si>
+  <si>
+    <t>字符串参数“{0}”不允许为 NULL 或空格符。</t>
   </si>
 </sst>
 </file>
@@ -1398,14 +1416,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="28.3" customHeight="1"/>
@@ -1803,6 +1821,46 @@
         <v>59</v>
       </c>
     </row>
+    <row r="19" customHeight="1" spans="1:9">
+      <c r="A19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" customHeight="1" spans="1:9">
+      <c r="A20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" sort="0" autoFilter="0"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
chore: 修改了 Excel 文件。
</commit_message>
<xml_diff>
--- a/assets/Localization-Resources.xlsx
+++ b/assets/Localization-Resources.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="69">
   <si>
     <t>Project</t>
   </si>
@@ -225,6 +225,15 @@
   </si>
   <si>
     <t>字符串参数“{0}”不允许为 NULL 或空格符。</t>
+  </si>
+  <si>
+    <t>ArgumentOutOfRangeException_invalid_network_port</t>
+  </si>
+  <si>
+    <t>Invalid network port number "{0}". The port number must be an integer value between 0 ~ 65535.</t>
+  </si>
+  <si>
+    <t>无效的网络端口号“{0}”。端口号必须是一个介于 0 ~ 65535 之间的整型值。</t>
   </si>
 </sst>
 </file>
@@ -1416,14 +1425,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I20" sqref="I20"/>
+      <selection pane="bottomRight" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="28.3" customHeight="1"/>
@@ -1861,6 +1870,26 @@
         <v>65</v>
       </c>
     </row>
+    <row r="21" customHeight="1" spans="1:9">
+      <c r="A21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" sort="0" autoFilter="0"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>